<commit_message>
added checking proccess for name persons
</commit_message>
<xml_diff>
--- a/hog-stud-report.xlsx
+++ b/hog-stud-report.xlsx
@@ -401,7 +401,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -458,16 +458,120 @@
         <v>44749.669333425925</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Анна</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3" t="str">
+        <v>https://vk.com/id739914548</v>
+      </c>
+      <c r="H3" s="1">
+        <v>44758.78654422454</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Олеся Грейнджер</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4" t="str">
+        <v>https://vk.com/id445175392</v>
+      </c>
+      <c r="H4" s="1">
+        <v>44758.81101667824</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Алекса Черни</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5" t="str">
+        <v>https://vk.com/id576527766</v>
+      </c>
+      <c r="H5" s="1">
+        <v>44759.35237075231</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="str">
+        <v>Иренчик</v>
+      </c>
+      <c r="C6">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6" t="str">
+        <v>https://vk.com/id332431318</v>
+      </c>
+      <c r="H6" s="1">
+        <v>44759.98855631945</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H6"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -524,16 +628,68 @@
         <v>44758.7337471412</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Делисия Ви-Марет</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+      <c r="G3" t="str">
+        <v>https://vk.com/id166767722</v>
+      </c>
+      <c r="H3" s="1">
+        <v>44758.81439315972</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Мак Так</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>6</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4" t="str">
+        <v>https://vk.com/id435298354</v>
+      </c>
+      <c r="H4" s="1">
+        <v>44759.710700891206</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H4"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -564,9 +720,87 @@
         <v>Дата регистрации</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="str">
+        <v>Драко Малфой</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>3</v>
+      </c>
+      <c r="G2" t="str">
+        <v>https://vk.com/id710936448</v>
+      </c>
+      <c r="H2" s="1">
+        <v>44758.80729621528</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Alhajia Unuk</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="F3">
+        <v>4</v>
+      </c>
+      <c r="G3" t="str">
+        <v>https://vk.com/id733827532</v>
+      </c>
+      <c r="H3" s="1">
+        <v>44758.935105150464</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Аделия Реддл</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4" t="str">
+        <v>https://vk.com/id391472095</v>
+      </c>
+      <c r="H4" s="1">
+        <v>44759.73308201389</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H4"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>